<commit_message>
temporal usage excel2016 as excel2019 and prepare office365 creation
</commit_message>
<xml_diff>
--- a/contents/office2019/excel/02/ichigo.xlsx
+++ b/contents/office2019/excel/02/ichigo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikot\Documents\大学　課題等\tutorleaders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e-learn\Desktop\excel2016 - コピー\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2492B6DF-990A-46B9-8C7A-122760FD1ED2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,6 +76,13 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>料金表(100g)</t>
+    <rPh sb="0" eb="3">
+      <t>リョウキンヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>上杉</t>
     <rPh sb="0" eb="2">
       <t>ウエスギ</t>
@@ -155,13 +161,6 @@
     <t>村上</t>
     <rPh sb="0" eb="2">
       <t>ムラカミ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>料金表(1g)</t>
-    <rPh sb="0" eb="3">
-      <t>リョウキンヒョウ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -169,10 +168,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
-    <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0.0;&quot;¥&quot;\-#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -260,21 +258,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="5" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,7 +274,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -567,30 +562,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="7" width="13.09765625" customWidth="1"/>
+    <col min="3" max="7" width="13.125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -608,15 +603,15 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
         <v>98</v>
@@ -627,18 +622,18 @@
       <c r="E3">
         <v>112</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="I3" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C4">
         <v>394</v>
@@ -649,18 +644,18 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="I4" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C5">
         <v>123</v>
@@ -671,18 +666,18 @@
       <c r="E5">
         <v>233</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="6" t="s">
         <v>14</v>
+      </c>
+      <c r="I5" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C6">
         <v>96</v>
@@ -693,12 +688,12 @@
       <c r="E6">
         <v>132</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -709,12 +704,12 @@
       <c r="E7">
         <v>197</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C8">
         <v>178</v>
@@ -725,12 +720,12 @@
       <c r="E8">
         <v>193</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -741,12 +736,12 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C10">
         <v>132</v>
@@ -757,12 +752,12 @@
       <c r="E10">
         <v>66</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C11">
         <v>245</v>
@@ -773,12 +768,12 @@
       <c r="E11">
         <v>78</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C12">
         <v>239</v>
@@ -789,12 +784,12 @@
       <c r="E12">
         <v>53</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="G13" s="2"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="G13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>